<commit_message>
Gestion UI de backup
Ajout la possibilité de mettre un backup dans la liste ainsi de le
supprimer.

Ajout de la validation des paramètres de backup.

Ajout de la liste de backup dans le programme principal
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinid223\Dropbox\Drive\Université\Hivers 2017\Processus concurrents et parallélisme - IFT630\TP\Projet\ProjectBackup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vinid223\Documents\Dropbox\Drive\Université\Hivers 2017\Processus concurrents et parallélisme - IFT630\TP\Projet\ProjectBackup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>14h30</t>
   </si>
@@ -33,6 +33,30 @@
   </si>
   <si>
     <t>Début de la configuration du projet qui consiste a créer le répertoire Git ainsi que de créer la solution Visual Studio du projet. Pour commencer dans le projet, j'ai définit une interface de base ainsi qu'une classe principal qui va servir de gestion des threads d'un backup. J'ai ensuite défénit chacune des classes nécessaire au threading du backup : FileWatch qui ferait la gestion de surveillange d'un répertoire, FileDiffEvaluator qui permet de déterminer si la différence est suffisante pour faire une nouvelle copie et FIleCopy qui permet de faire la copie selon les paramètres de l'application</t>
+  </si>
+  <si>
+    <t>18h00</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Heure Début</t>
+  </si>
+  <si>
+    <t>Heure Fin</t>
+  </si>
+  <si>
+    <t>Temps total (minutes)</t>
+  </si>
+  <si>
+    <t>Description du travail</t>
+  </si>
+  <si>
+    <t>23h00</t>
+  </si>
+  <si>
+    <t>Création de l'objet de backup et défénition complete de l'affichage des informations du backup. Ajout de la validation des informations du backup. Ajout d'une fenêtre de création de backup. Modelisation de l'affichage général</t>
   </si>
 </sst>
 </file>
@@ -68,11 +92,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -388,79 +418,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:O11"/>
+  <dimension ref="B2:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+    </row>
+    <row r="3" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>42811</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="F3">
+        <v>45</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -469,40 +565,112 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>42822</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>300</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+    </row>
+    <row r="13" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="H3:O11"/>
+  <mergeCells count="3">
+    <mergeCell ref="H9:U13"/>
+    <mergeCell ref="H3:U7"/>
+    <mergeCell ref="H2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Transfert fonctionnel, mais supprimer la gestion de répétitin car non fonctionnel
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>14h30</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Implémentation simple du watcher</t>
+  </si>
+  <si>
+    <t>15h00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implémentation d'un logger pour avoir des informations et feedback plus parlant. Ajout de la copie de fichier selon le changement ainsi que la suppression de fichier lorsqu'il disparait. Ajout de la gestion d'Erreur de fichier. Ajout de la répétition des opérations lorsd'une erreur jusqu'a un nombre de répétition. </t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Z19"/>
+  <dimension ref="B2:Z25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="H21" sqref="H21:U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,15 +529,15 @@
       <c r="U3" s="3"/>
       <c r="X3">
         <f>SUM(F3:F196)</f>
-        <v>360</v>
+        <v>510</v>
       </c>
       <c r="Y3">
         <f>X3/60</f>
-        <v>6</v>
+        <v>8.5</v>
       </c>
       <c r="Z3">
         <f>30-Y3</f>
-        <v>24</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
@@ -754,7 +760,7 @@
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
     </row>
-    <row r="17" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -770,7 +776,7 @@
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
     </row>
-    <row r="18" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -786,7 +792,7 @@
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
     </row>
-    <row r="19" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
@@ -802,12 +808,107 @@
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
     </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>42825</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21">
+        <v>150</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="H9:U13"/>
     <mergeCell ref="H3:U7"/>
     <mergeCell ref="H2:U2"/>
     <mergeCell ref="H15:U19"/>
+    <mergeCell ref="H21:U25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correction buffer, correction wait
Il faut faire une implémentation de thread pour chaque appels du watcher
pour éviter de perdre des évènements
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinid223\Dropbox\Drive\Université\Hivers 2017\Processus concurrents et parallélisme - IFT630\TP\Projet\ProjectBackup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vinid223\Documents\Dropbox\Drive\Université\Hivers 2017\Processus concurrents et parallélisme - IFT630\TP\Projet\ProjectBackup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>14h30</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t xml:space="preserve">Implémentation d'un logger pour avoir des informations et feedback plus parlant. Ajout de la copie de fichier selon le changement ainsi que la suppression de fichier lorsqu'il disparait. Ajout de la gestion d'Erreur de fichier. Ajout de la répétition des opérations lorsd'une erreur jusqu'a un nombre de répétition. </t>
+  </si>
+  <si>
+    <t>2-avr-17</t>
+  </si>
+  <si>
+    <t>10h30</t>
+  </si>
+  <si>
+    <t>11h30</t>
   </si>
 </sst>
 </file>
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Z25"/>
+  <dimension ref="B2:Z27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:U25"/>
+      <selection activeCell="H28" sqref="H28:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,15 +538,15 @@
       <c r="U3" s="3"/>
       <c r="X3">
         <f>SUM(F3:F196)</f>
-        <v>510</v>
+        <v>570</v>
       </c>
       <c r="Y3">
         <f>X3/60</f>
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="Z3">
         <f>30-Y3</f>
-        <v>21.5</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
@@ -902,6 +911,20 @@
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
     </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="H9:U13"/>

</xml_diff>

<commit_message>
Changement gestion exception et logger + timesheet
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>14h30</t>
   </si>
@@ -89,7 +89,10 @@
     <t>10h30</t>
   </si>
   <si>
-    <t>11h30</t>
+    <t>11h45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correction du buffer du watcher. Implémentation d'une meilleur gestion de lock sur les fichiers. </t>
   </si>
 </sst>
 </file>
@@ -451,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Z27"/>
+  <dimension ref="B2:Z31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28:I28"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,15 +541,15 @@
       <c r="U3" s="3"/>
       <c r="X3">
         <f>SUM(F3:F196)</f>
-        <v>570</v>
+        <v>585</v>
       </c>
       <c r="Y3">
         <f>X3/60</f>
-        <v>9.5</v>
+        <v>9.75</v>
       </c>
       <c r="Z3">
         <f>30-Y3</f>
-        <v>20.5</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
@@ -922,11 +925,92 @@
         <v>21</v>
       </c>
       <c r="F27">
-        <v>60</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="H27:U31"/>
     <mergeCell ref="H9:U13"/>
     <mergeCell ref="H3:U7"/>
     <mergeCell ref="H2:U2"/>

</xml_diff>

<commit_message>
Ajout de thread pour chaque actions de fichiers et remodelage du code
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>14h30</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t xml:space="preserve">Correction du buffer du watcher. Implémentation d'une meilleur gestion de lock sur les fichiers. </t>
+  </si>
+  <si>
+    <t>11h00</t>
+  </si>
+  <si>
+    <t>12h00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout de thread pour chaque opérations. </t>
   </si>
 </sst>
 </file>
@@ -454,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Z31"/>
+  <dimension ref="B2:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33:U37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,15 +550,15 @@
       <c r="U3" s="3"/>
       <c r="X3">
         <f>SUM(F3:F196)</f>
-        <v>585</v>
+        <v>645</v>
       </c>
       <c r="Y3">
         <f>X3/60</f>
-        <v>9.75</v>
+        <v>10.75</v>
       </c>
       <c r="Z3">
         <f>30-Y3</f>
-        <v>20.25</v>
+        <v>19.25</v>
       </c>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
@@ -1008,8 +1017,103 @@
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
     </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33">
+        <v>60</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="H33:U37"/>
     <mergeCell ref="H27:U31"/>
     <mergeCell ref="H9:U13"/>
     <mergeCell ref="H3:U7"/>

</xml_diff>

<commit_message>
Deplacement de fichiers, ajout sauvegarde des backups
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>14h30</t>
   </si>
@@ -101,7 +101,19 @@
     <t>12h00</t>
   </si>
   <si>
-    <t xml:space="preserve">Ajout de thread pour chaque opérations. </t>
+    <t>3-avr-17</t>
+  </si>
+  <si>
+    <t>9h00</t>
+  </si>
+  <si>
+    <t>13h00</t>
+  </si>
+  <si>
+    <t>Ajout de thread pour chaque opérations. Corrections problème de mass transfert</t>
+  </si>
+  <si>
+    <t>Ajout d'un fichier de configuration xml permettant de garder sur disque la liste des backups pour les charger au démarage de l'application.</t>
   </si>
 </sst>
 </file>
@@ -463,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Z37"/>
+  <dimension ref="B2:Z44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33:U37"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="V39" sqref="V39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,15 +562,15 @@
       <c r="U3" s="3"/>
       <c r="X3">
         <f>SUM(F3:F196)</f>
-        <v>645</v>
+        <v>885</v>
       </c>
       <c r="Y3">
         <f>X3/60</f>
-        <v>10.75</v>
+        <v>14.75</v>
       </c>
       <c r="Z3">
         <f>30-Y3</f>
-        <v>19.25</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
@@ -1031,7 +1043,7 @@
         <v>60</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
@@ -1111,8 +1123,103 @@
       <c r="T37" s="3"/>
       <c r="U37" s="3"/>
     </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40">
+        <v>240</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="3"/>
+      <c r="U41" s="3"/>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="U44" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="H40:U44"/>
     <mergeCell ref="H33:U37"/>
     <mergeCell ref="H27:U31"/>
     <mergeCell ref="H9:U13"/>

</xml_diff>

<commit_message>
Changement buffer pour une plus grande valeur, ajout du début du rapport
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinid223\Dropbox\Drive\Université\Hivers 2017\Processus concurrents et parallélisme - IFT630\TP\Projet\ProjectBackup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vinid223\Documents\Dropbox\Drive\Université\Hivers 2017\Processus concurrents et parallélisme - IFT630\TP\Projet\ProjectBackup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>14h30</t>
   </si>
@@ -123,6 +123,24 @@
   </si>
   <si>
     <t xml:space="preserve">Ajout de la copie parallele de tout un dossier source lors de l'initialisation d'un backup. Correction de problème avec le fichier de configuration. Ajout de la gestion de copier les fichiers change lorsque le programme ou le watcher ne fonctionnait pas. Ajout de la gestion du fichier de controle dans le dossier de destination. Correction de certain problèmes. </t>
+  </si>
+  <si>
+    <t>5-avr-17</t>
+  </si>
+  <si>
+    <t>16h00</t>
+  </si>
+  <si>
+    <t>17h00</t>
+  </si>
+  <si>
+    <t>20h30</t>
+  </si>
+  <si>
+    <t>22h00</t>
+  </si>
+  <si>
+    <t>Finalisation de certain commentaire et restructuration d'appels de certaines méthodes. Début du rapport.</t>
   </si>
 </sst>
 </file>
@@ -484,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Z50"/>
+  <dimension ref="B2:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46:U50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,15 +589,15 @@
       <c r="U3" s="3"/>
       <c r="X3">
         <f>SUM(F3:F196)</f>
-        <v>1065</v>
+        <v>1215</v>
       </c>
       <c r="Y3">
         <f>X3/60</f>
-        <v>17.75</v>
+        <v>20.25</v>
       </c>
       <c r="Z3">
         <f>30-Y3</f>
-        <v>12.25</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
@@ -1288,7 +1306,7 @@
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
     </row>
-    <row r="49" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
@@ -1304,7 +1322,7 @@
       <c r="T49" s="3"/>
       <c r="U49" s="3"/>
     </row>
-    <row r="50" spans="8:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
@@ -1320,8 +1338,112 @@
       <c r="T50" s="3"/>
       <c r="U50" s="3"/>
     </row>
+    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52">
+        <v>60</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+      <c r="U52" s="3"/>
+    </row>
+    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53" t="s">
+        <v>37</v>
+      </c>
+      <c r="F53">
+        <v>90</v>
+      </c>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="T53" s="3"/>
+      <c r="U53" s="3"/>
+    </row>
+    <row r="54" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3"/>
+      <c r="R54" s="3"/>
+      <c r="S54" s="3"/>
+      <c r="T54" s="3"/>
+      <c r="U54" s="3"/>
+    </row>
+    <row r="55" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="3"/>
+      <c r="P55" s="3"/>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="3"/>
+      <c r="U55" s="3"/>
+    </row>
+    <row r="56" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="3"/>
+      <c r="U56" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="H52:U56"/>
     <mergeCell ref="H46:U50"/>
     <mergeCell ref="H2:U2"/>
     <mergeCell ref="H15:U19"/>

</xml_diff>

<commit_message>
Changement de la time sheet
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vinid223\Documents\Dropbox\Drive\Université\Hivers 2017\Processus concurrents et parallélisme - IFT630\TP\Projet\ProjectBackup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinid223\Dropbox\Drive\Université\Hivers 2017\Processus concurrents et parallélisme - IFT630\TP\Projet\ProjectBackup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>14h30</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>Finalisation de certain commentaire et restructuration d'appels de certaines méthodes. Début du rapport.</t>
+  </si>
+  <si>
+    <t>6-avr-17</t>
+  </si>
+  <si>
+    <t>14h00</t>
+  </si>
+  <si>
+    <t>Continuité du rapport et changement de certains paramètres de l'application.</t>
   </si>
 </sst>
 </file>
@@ -502,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Z56"/>
+  <dimension ref="B2:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="W56" sqref="W56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,15 +598,15 @@
       <c r="U3" s="3"/>
       <c r="X3">
         <f>SUM(F3:F196)</f>
-        <v>1215</v>
+        <v>1305</v>
       </c>
       <c r="Y3">
         <f>X3/60</f>
-        <v>20.25</v>
+        <v>21.75</v>
       </c>
       <c r="Z3">
         <f>30-Y3</f>
-        <v>9.75</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
@@ -1441,8 +1450,103 @@
       <c r="T56" s="3"/>
       <c r="U56" s="3"/>
     </row>
+    <row r="58" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>39</v>
+      </c>
+      <c r="D58" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58">
+        <v>90</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3"/>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+    </row>
+    <row r="59" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="3"/>
+      <c r="T59" s="3"/>
+      <c r="U59" s="3"/>
+    </row>
+    <row r="60" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="3"/>
+      <c r="T60" s="3"/>
+      <c r="U60" s="3"/>
+    </row>
+    <row r="61" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="3"/>
+      <c r="T61" s="3"/>
+      <c r="U61" s="3"/>
+    </row>
+    <row r="62" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="3"/>
+      <c r="T62" s="3"/>
+      <c r="U62" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="H58:U62"/>
     <mergeCell ref="H52:U56"/>
     <mergeCell ref="H46:U50"/>
     <mergeCell ref="H2:U2"/>

</xml_diff>

<commit_message>
Corrections problèmes globals, suppression fichier offline
Corrections de certain problèmes de watch ainsi que l'ajout de la
possibilité de supprimer des fichiers dans le répertoire de destination
lorsque le watcher ou l'application central n'était pas en exécution.
Correction et fin de l'implémentation des boutons play et pauses pour
les watchers.
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>14h30</t>
   </si>
@@ -150,6 +150,21 @@
   </si>
   <si>
     <t>Continuité du rapport et changement de certains paramètres de l'application.</t>
+  </si>
+  <si>
+    <t>9-avr-17</t>
+  </si>
+  <si>
+    <t>Ajout de la gestion des fichiers supprimé du dossier source lorsque le watcher n'est pas en route. Ajout du traitement en parallèle lors de l'ajout d'une nouvelle sauvegarde et de la réouverture du programme pour faire le traitement en parallèle de chacune des sauvegardes.</t>
+  </si>
+  <si>
+    <t>23h45</t>
+  </si>
+  <si>
+    <t>10-avr-17</t>
+  </si>
+  <si>
+    <t>Verification et tests de performance global. Corrections de certains problèmes. Fin de l'implémentation des boutons play et pause du watcher. Finalisation du document.</t>
   </si>
 </sst>
 </file>
@@ -511,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Z62"/>
+  <dimension ref="B2:Z75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="W56" sqref="W56"/>
+    <sheetView tabSelected="1" topLeftCell="C53" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,15 +613,15 @@
       <c r="U3" s="3"/>
       <c r="X3">
         <f>SUM(F3:F196)</f>
-        <v>1305</v>
+        <v>1500</v>
       </c>
       <c r="Y3">
         <f>X3/60</f>
-        <v>21.75</v>
+        <v>25</v>
       </c>
       <c r="Z3">
         <f>30-Y3</f>
-        <v>8.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
@@ -1544,8 +1559,198 @@
       <c r="T62" s="3"/>
       <c r="U62" s="3"/>
     </row>
+    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>42</v>
+      </c>
+      <c r="D65" t="s">
+        <v>37</v>
+      </c>
+      <c r="E65" t="s">
+        <v>44</v>
+      </c>
+      <c r="F65">
+        <v>105</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="3"/>
+      <c r="T65" s="3"/>
+      <c r="U65" s="3"/>
+    </row>
+    <row r="66" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="3"/>
+      <c r="T66" s="3"/>
+      <c r="U66" s="3"/>
+    </row>
+    <row r="67" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="3"/>
+      <c r="T67" s="3"/>
+      <c r="U67" s="3"/>
+    </row>
+    <row r="68" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="3"/>
+      <c r="T68" s="3"/>
+      <c r="U68" s="3"/>
+    </row>
+    <row r="69" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3"/>
+      <c r="N69" s="3"/>
+      <c r="O69" s="3"/>
+      <c r="P69" s="3"/>
+      <c r="Q69" s="3"/>
+      <c r="R69" s="3"/>
+      <c r="S69" s="3"/>
+      <c r="T69" s="3"/>
+      <c r="U69" s="3"/>
+    </row>
+    <row r="71" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>45</v>
+      </c>
+      <c r="D71" t="s">
+        <v>14</v>
+      </c>
+      <c r="E71" t="s">
+        <v>40</v>
+      </c>
+      <c r="F71">
+        <v>90</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="3"/>
+      <c r="O71" s="3"/>
+      <c r="P71" s="3"/>
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="3"/>
+      <c r="T71" s="3"/>
+      <c r="U71" s="3"/>
+    </row>
+    <row r="72" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+      <c r="M72" s="3"/>
+      <c r="N72" s="3"/>
+      <c r="O72" s="3"/>
+      <c r="P72" s="3"/>
+      <c r="Q72" s="3"/>
+      <c r="R72" s="3"/>
+      <c r="S72" s="3"/>
+      <c r="T72" s="3"/>
+      <c r="U72" s="3"/>
+    </row>
+    <row r="73" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="3"/>
+      <c r="P73" s="3"/>
+      <c r="Q73" s="3"/>
+      <c r="R73" s="3"/>
+      <c r="S73" s="3"/>
+      <c r="T73" s="3"/>
+      <c r="U73" s="3"/>
+    </row>
+    <row r="74" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="3"/>
+      <c r="N74" s="3"/>
+      <c r="O74" s="3"/>
+      <c r="P74" s="3"/>
+      <c r="Q74" s="3"/>
+      <c r="R74" s="3"/>
+      <c r="S74" s="3"/>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+    </row>
+    <row r="75" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
+      <c r="P75" s="3"/>
+      <c r="Q75" s="3"/>
+      <c r="R75" s="3"/>
+      <c r="S75" s="3"/>
+      <c r="T75" s="3"/>
+      <c r="U75" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="H71:U75"/>
+    <mergeCell ref="H65:U69"/>
     <mergeCell ref="H58:U62"/>
     <mergeCell ref="H52:U56"/>
     <mergeCell ref="H46:U50"/>

</xml_diff>